<commit_message>
creacion de las deficiniciones de las rutas y archivo de especificaciones (incompleto)
</commit_message>
<xml_diff>
--- a/peticiones.xlsx
+++ b/peticiones.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -129,7 +129,7 @@
     <t xml:space="preserve">subir archivo de datos</t>
   </si>
   <si>
-    <t xml:space="preserve">/datos/?version</t>
+    <t xml:space="preserve">/archivo/?version</t>
   </si>
   <si>
     <t xml:space="preserve">sube un conjunto de datos al servidor especificando la version del archivo de configuracion</t>
@@ -153,6 +153,178 @@
   </si>
   <si>
     <t xml:space="preserve">obtiene el archivo de datos de la version especificada desde el servidor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regresa_archivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guardar (cambiar nombre a archivo) archivo de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/archivo/guardar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">guarda el archivo de datos con un nombre especificado por el usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+archivo_anterior: “nombre_archivo”,
+archivo_nuevo: “nombre_archivo”
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ status: ok, 
+mensaje: “guardado con exito”
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crear instancia (nueva fila de datos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/datos/?version/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crea un nuevo objeto en el archivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+objeto: objeto
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modificar instancia (modificar algun valor o valores de la fila)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modifica un objeto en el archivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+id: id,
+objeto: objeto
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ status: ok, 
+mensaje: “modificado con exito”
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eliminar instancia (eliminar algun objeto (fila) del archivo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/archivo/?version/?id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elimina un objeto completo del archivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">version,id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ status: ok, 
+mensaje: “eliminado con exito”
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revisar el archivo de especificaciones para ver exactamente como esta constituido el id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agregar atributo (columna completa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/archivo/?version/atributo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">crea una columna completa en todos los datos (con el valor especificado como sin valor)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+nombre_atributo: “nombre”
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eliminar atributo (columna  completa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/archivo/?version/atributo/?nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elimina una columna completa (en todos los objetos del archivo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">version, nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtener bases de datos disponibles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/base-de-datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtiene el nombre de las bases de datos disponibles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ status: ok, 
+bases: [“nombre1”, “nombre2”, “etc”]
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtener tablas de las bases de datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/base-de-datos/?nombre/tablas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtiene el nombre de las tablas de la base de datos especificada </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ status: ok, 
+tablas: [“nombre1”, “nombre2”, “etc”]
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtener atributos de la tabla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/base-de-datos/?nombre/tablas/?nombre-tabla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtiene la lista de los atributos de la tabla especificada de la base de datos especificada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre, nombre-tabla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ status: ok, 
+atributos: [“nombre1”, “nombre2”, “etc”]
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtener datos de la tabla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/base-de-datos/?nombre/?nombre-tabla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtiene los datos de  la tabla especificada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{
+ status: ok, 
+datos: objeto_tipo_datos
+}</t>
   </si>
 </sst>
 </file>
@@ -162,11 +334,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -188,6 +361,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -232,7 +413,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -246,6 +427,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -266,18 +451,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.93"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="19.17"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="2" width="11.52"/>
@@ -406,7 +592,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -432,7 +618,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
@@ -447,6 +633,229 @@
       </c>
       <c r="E8" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creado esqueleto de la api, creado coleccion de postman, se modificaron algunas rutas
</commit_message>
<xml_diff>
--- a/peticiones.xlsx
+++ b/peticiones.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="86">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -357,14 +357,14 @@
       <family val="0"/>
     </font>
     <font>
-      <i val="true"/>
+      <u val="single"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -413,7 +413,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -427,10 +427,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -453,8 +457,8 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -539,6 +543,10 @@
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3"/>
       <c r="G4" s="1" t="s">
         <v>16</v>
       </c>
@@ -596,7 +604,7 @@
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -622,7 +630,7 @@
       <c r="A8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -660,7 +668,7 @@
       <c r="G9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
@@ -776,7 +784,7 @@
       <c r="E14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="1" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
eliminado el archivo temporal de excel
</commit_message>
<xml_diff>
--- a/peticiones.xlsx
+++ b/peticiones.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="85">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -158,24 +158,18 @@
     <t xml:space="preserve">regresa_archivo</t>
   </si>
   <si>
-    <t xml:space="preserve">guardar (cambiar nombre a archivo) archivo de datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/archivo/guardar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">guarda el archivo de datos con un nombre especificado por el usuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{
-archivo_anterior: “nombre_archivo”,
-archivo_nuevo: “nombre_archivo”
-}</t>
+    <t xml:space="preserve">obtener datos del objeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/datos/?version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regresa todos los datos en formato json</t>
   </si>
   <si>
     <t xml:space="preserve">{
  status: ok, 
-mensaje: “guardado con exito”
+datos: [{objeto_datos}]
 }</t>
   </si>
   <si>
@@ -214,7 +208,7 @@
     <t xml:space="preserve">eliminar instancia (eliminar algun objeto (fila) del archivo)</t>
   </si>
   <si>
-    <t xml:space="preserve">/archivo/?version/?id</t>
+    <t xml:space="preserve">/datos/?version/?id</t>
   </si>
   <si>
     <t xml:space="preserve">elimina un objeto completo del archivo</t>
@@ -238,7 +232,7 @@
     <t xml:space="preserve">agregar atributo (columna completa)</t>
   </si>
   <si>
-    <t xml:space="preserve">/archivo/?version/atributo</t>
+    <t xml:space="preserve">/datos/?version/atributo</t>
   </si>
   <si>
     <t xml:space="preserve">crea una columna completa en todos los datos (con el valor especificado como sin valor)</t>
@@ -252,7 +246,7 @@
     <t xml:space="preserve">eliminar atributo (columna  completa)</t>
   </si>
   <si>
-    <t xml:space="preserve">/archivo/?version/atributo/?nombre</t>
+    <t xml:space="preserve">/datos/?version/atributo/?nombre</t>
   </si>
   <si>
     <t xml:space="preserve">elimina una columna completa (en todos los objetos del archivo)</t>
@@ -457,8 +451,8 @@
   </sheetPr>
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -649,36 +643,35 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="1" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>34</v>
@@ -687,7 +680,7 @@
         <v>23</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>36</v>
@@ -696,15 +689,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>28</v>
@@ -713,10 +706,10 @@
         <v>23</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>25</v>
@@ -724,36 +717,36 @@
     </row>
     <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H12" s="1" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>34</v>
@@ -762,108 +755,108 @@
         <v>23</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="1" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="G16" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="1" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="G17" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G17" s="1" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>